<commit_message>
tinkering with adding subs list
</commit_message>
<xml_diff>
--- a/data/monetary/M_1008.xlsx
+++ b/data/monetary/M_1008.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswyngaarden/Documents/GitHub/istart-effort/data/monetary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BAFC860-C2AA-4540-AAA8-06366CA8582D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95DB9DC-A922-0649-B006-C68ECE12B880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20740" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2800" yWindow="2740" windowWidth="20740" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="M_1008" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="36">
   <si>
     <t>ExperimentName</t>
   </si>
@@ -116,6 +116,18 @@
   </si>
   <si>
     <t>Win</t>
+  </si>
+  <si>
+    <t>AmtWon</t>
+  </si>
+  <si>
+    <t>Clock.Information</t>
+  </si>
+  <si>
+    <t>EasyKey</t>
+  </si>
+  <si>
+    <t>ExperimentVersion</t>
   </si>
 </sst>
 </file>
@@ -962,38 +974,38 @@
   <dimension ref="A1:AI68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="A1:I68"/>
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A1">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>0</v>
-      </c>
-      <c r="D1">
-        <v>0</v>
-      </c>
-      <c r="E1">
-        <v>0</v>
-      </c>
-      <c r="F1">
-        <v>0</v>
-      </c>
-      <c r="G1">
-        <v>0</v>
-      </c>
-      <c r="H1">
-        <v>0</v>
-      </c>
-      <c r="I1">
-        <v>0</v>
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
+        <v>35</v>
       </c>
       <c r="J1" t="s">
         <v>0</v>

</xml_diff>